<commit_message>
questionnair Analysis, chapter one and two
</commit_message>
<xml_diff>
--- a/MSc Work/questionnaire_analysis.xlsx
+++ b/MSc Work/questionnaire_analysis.xlsx
@@ -1396,6 +1396,10 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="13" fillId="3" borderId="3" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1420,10 +1424,6 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="3" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,20 +1437,21 @@
     <cellStyle name="Normal 6" xfId="7"/>
     <cellStyle name="Normal 7" xfId="8"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCFF"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1479,21 +1480,6 @@
           <bgColor rgb="FFFFCCFF"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1625,13 +1611,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3225,13 +3211,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3819,16 +3805,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4426,16 +4412,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -6142,16 +6128,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -6341,16 +6327,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -6938,13 +6924,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -7535,16 +7521,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -7734,16 +7720,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -11573,7 +11559,7 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E44" sqref="E44"/>
+      <selection pane="topRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11590,11 +11576,11 @@
       <c r="B2" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="H2" s="115" t="s">
+      <c r="H2" s="116" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
     </row>
     <row r="3" spans="1:115" x14ac:dyDescent="0.25">
       <c r="D3" s="7"/>
@@ -11635,7 +11621,7 @@
       <c r="C5" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="123">
+      <c r="D5" s="115">
         <v>43667</v>
       </c>
       <c r="E5" s="76"/>
@@ -11747,13 +11733,13 @@
     </row>
     <row r="10" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="119" t="s">
+      <c r="B10" s="120" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="121"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="122"/>
       <c r="G10" s="20" t="s">
         <v>104</v>
       </c>
@@ -12066,14 +12052,14 @@
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="116">
+      <c r="B11" s="117">
         <f>H3</f>
         <v>0</v>
       </c>
-      <c r="C11" s="117"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="118"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="119"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
@@ -12186,14 +12172,14 @@
       <c r="A12" s="16">
         <v>2</v>
       </c>
-      <c r="B12" s="116">
+      <c r="B12" s="117">
         <f>I3</f>
         <v>0</v>
       </c>
-      <c r="C12" s="117"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="117"/>
-      <c r="F12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="119"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -12306,14 +12292,14 @@
       <c r="A13" s="16">
         <v>3</v>
       </c>
-      <c r="B13" s="116">
+      <c r="B13" s="117">
         <f>J3</f>
         <v>0</v>
       </c>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
-      <c r="F13" s="118"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="118"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="119"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -12434,13 +12420,13 @@
     </row>
     <row r="14" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
-      <c r="B14" s="119" t="s">
+      <c r="B14" s="120" t="s">
         <v>122</v>
       </c>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="121"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="122"/>
       <c r="G14" s="105"/>
       <c r="H14" s="106"/>
       <c r="I14" s="106"/>
@@ -12584,7 +12570,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I15" s="13">
         <v>4</v>
@@ -12602,13 +12588,13 @@
         <v>3</v>
       </c>
       <c r="N15" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O15" s="13">
         <v>3</v>
       </c>
       <c r="P15" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q15" s="13">
         <v>3</v>
@@ -12704,7 +12690,7 @@
       <c r="DB15" s="13"/>
       <c r="DC15" s="14">
         <f>IF(ISERROR(AVERAGE(G15:DB15)),"",AVERAGE(G15:DB15))</f>
-        <v>3.4545454545454546</v>
+        <v>3.8181818181818183</v>
       </c>
       <c r="DD15" s="15">
         <f t="shared" ref="DD15:DD41" si="0">COUNT(G15:DB15)</f>
@@ -12712,15 +12698,15 @@
       </c>
       <c r="DE15" s="28">
         <f t="shared" ref="DE15:DE41" si="1">COUNTIF(G15:DB15,5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DF15" s="28">
         <f t="shared" ref="DF15:DF41" si="2">COUNTIF(G15:DB15,4)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="DG15" s="28">
         <f t="shared" ref="DG15:DG41" si="3">COUNTIF(G15:DB15,3)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="DH15" s="28">
         <f t="shared" ref="DH15:DH41" si="4">COUNTIF(G15:DB15,2)</f>
@@ -12732,7 +12718,7 @@
       </c>
       <c r="DJ15" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE15+'Questionnaire Analysis Sheet'!DF15)/'Questionnaire Analysis Sheet'!DD15),"",('Questionnaire Analysis Sheet'!DE15+'Questionnaire Analysis Sheet'!DF15)/'Questionnaire Analysis Sheet'!DD15)</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="DK15" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH15+'Questionnaire Analysis Sheet'!DI15)/'Questionnaire Analysis Sheet'!DD15),"",('Questionnaire Analysis Sheet'!DH15+'Questionnaire Analysis Sheet'!DI15)/'Questionnaire Analysis Sheet'!DD15)</f>
@@ -12757,19 +12743,19 @@
         <v>5</v>
       </c>
       <c r="I16" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16" s="13">
         <v>3</v>
       </c>
       <c r="K16" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L16" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M16" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N16" s="13">
         <v>3</v>
@@ -12874,7 +12860,7 @@
       <c r="DB16" s="13"/>
       <c r="DC16" s="14">
         <f t="shared" ref="DC16:DC41" si="6">IF(ISERROR(AVERAGE(G16:DB16)),"",AVERAGE(G16:DB16))</f>
-        <v>3.4545454545454546</v>
+        <v>4.0909090909090908</v>
       </c>
       <c r="DD16" s="15">
         <f t="shared" si="0"/>
@@ -12882,19 +12868,19 @@
       </c>
       <c r="DE16" s="28">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="DF16" s="28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DG16" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="DH16" s="28">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DI16" s="28">
         <f t="shared" si="5"/>
@@ -12902,11 +12888,11 @@
       </c>
       <c r="DJ16" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE16+'Questionnaire Analysis Sheet'!DF16)/'Questionnaire Analysis Sheet'!DD16),"",('Questionnaire Analysis Sheet'!DE16+'Questionnaire Analysis Sheet'!DF16)/'Questionnaire Analysis Sheet'!DD16)</f>
-        <v>0.45454545454545453</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="DK16" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH16+'Questionnaire Analysis Sheet'!DI16)/'Questionnaire Analysis Sheet'!DD16),"",('Questionnaire Analysis Sheet'!DH16+'Questionnaire Analysis Sheet'!DI16)/'Questionnaire Analysis Sheet'!DD16)</f>
-        <v>0.18181818181818182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -12924,7 +12910,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" s="13">
         <v>4</v>
@@ -12933,7 +12919,7 @@
         <v>4</v>
       </c>
       <c r="K17" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L17" s="13">
         <v>3</v>
@@ -13044,7 +13030,7 @@
       <c r="DB17" s="13"/>
       <c r="DC17" s="14">
         <f t="shared" si="6"/>
-        <v>3.3636363636363638</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="DD17" s="15">
         <f t="shared" si="0"/>
@@ -13052,19 +13038,19 @@
       </c>
       <c r="DE17" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DF17" s="28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DG17" s="28">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="DH17" s="28">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI17" s="28">
         <f t="shared" si="5"/>
@@ -13072,11 +13058,11 @@
       </c>
       <c r="DJ17" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE17+'Questionnaire Analysis Sheet'!DF17)/'Questionnaire Analysis Sheet'!DD17),"",('Questionnaire Analysis Sheet'!DE17+'Questionnaire Analysis Sheet'!DF17)/'Questionnaire Analysis Sheet'!DD17)</f>
-        <v>0.36363636363636365</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="DK17" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH17+'Questionnaire Analysis Sheet'!DI17)/'Questionnaire Analysis Sheet'!DD17),"",('Questionnaire Analysis Sheet'!DH17+'Questionnaire Analysis Sheet'!DI17)/'Questionnaire Analysis Sheet'!DD17)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -13091,13 +13077,13 @@
       <c r="E18" s="89"/>
       <c r="F18" s="111"/>
       <c r="G18" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I18" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J18" s="13">
         <v>4</v>
@@ -13214,7 +13200,7 @@
       <c r="DB18" s="13"/>
       <c r="DC18" s="14">
         <f t="shared" si="6"/>
-        <v>3.5454545454545454</v>
+        <v>4</v>
       </c>
       <c r="DD18" s="15">
         <f t="shared" si="0"/>
@@ -13222,19 +13208,19 @@
       </c>
       <c r="DE18" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DF18" s="28">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="DG18" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="DH18" s="28">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI18" s="28">
         <f t="shared" si="5"/>
@@ -13242,11 +13228,11 @@
       </c>
       <c r="DJ18" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE18+'Questionnaire Analysis Sheet'!DF18)/'Questionnaire Analysis Sheet'!DD18),"",('Questionnaire Analysis Sheet'!DE18+'Questionnaire Analysis Sheet'!DF18)/'Questionnaire Analysis Sheet'!DD18)</f>
-        <v>0.54545454545454541</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="DK18" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH18+'Questionnaire Analysis Sheet'!DI18)/'Questionnaire Analysis Sheet'!DD18),"",('Questionnaire Analysis Sheet'!DH18+'Questionnaire Analysis Sheet'!DI18)/'Questionnaire Analysis Sheet'!DD18)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -13264,10 +13250,10 @@
         <v>4</v>
       </c>
       <c r="H19" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I19" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J19" s="13">
         <v>5</v>
@@ -13279,10 +13265,10 @@
         <v>3</v>
       </c>
       <c r="M19" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N19" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O19" s="13">
         <v>3</v>
@@ -13384,7 +13370,7 @@
       <c r="DB19" s="13"/>
       <c r="DC19" s="14">
         <f t="shared" si="6"/>
-        <v>3.4545454545454546</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="DD19" s="15">
         <f t="shared" si="0"/>
@@ -13392,15 +13378,15 @@
       </c>
       <c r="DE19" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="DF19" s="28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="DG19" s="28">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="DH19" s="28">
         <f t="shared" si="4"/>
@@ -13412,7 +13398,7 @@
       </c>
       <c r="DJ19" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE19+'Questionnaire Analysis Sheet'!DF19)/'Questionnaire Analysis Sheet'!DD19),"",('Questionnaire Analysis Sheet'!DE19+'Questionnaire Analysis Sheet'!DF19)/'Questionnaire Analysis Sheet'!DD19)</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="DK19" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH19+'Questionnaire Analysis Sheet'!DI19)/'Questionnaire Analysis Sheet'!DD19),"",('Questionnaire Analysis Sheet'!DH19+'Questionnaire Analysis Sheet'!DI19)/'Questionnaire Analysis Sheet'!DD19)</f>
@@ -13431,25 +13417,25 @@
       <c r="E20" s="89"/>
       <c r="F20" s="111"/>
       <c r="G20" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H20" s="13">
         <v>5</v>
       </c>
       <c r="I20" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J20" s="13">
         <v>3</v>
       </c>
       <c r="K20" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L20" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M20" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N20" s="13">
         <v>3</v>
@@ -13554,7 +13540,7 @@
       <c r="DB20" s="13"/>
       <c r="DC20" s="14">
         <f t="shared" si="6"/>
-        <v>3.4545454545454546</v>
+        <v>4.3636363636363633</v>
       </c>
       <c r="DD20" s="15">
         <f t="shared" si="0"/>
@@ -13562,7 +13548,7 @@
       </c>
       <c r="DE20" s="28">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="DF20" s="28">
         <f t="shared" si="2"/>
@@ -13570,11 +13556,11 @@
       </c>
       <c r="DG20" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="DH20" s="28">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DI20" s="28">
         <f t="shared" si="5"/>
@@ -13582,11 +13568,11 @@
       </c>
       <c r="DJ20" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE20+'Questionnaire Analysis Sheet'!DF20)/'Questionnaire Analysis Sheet'!DD20),"",('Questionnaire Analysis Sheet'!DE20+'Questionnaire Analysis Sheet'!DF20)/'Questionnaire Analysis Sheet'!DD20)</f>
-        <v>0.45454545454545453</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="DK20" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH20+'Questionnaire Analysis Sheet'!DI20)/'Questionnaire Analysis Sheet'!DD20),"",('Questionnaire Analysis Sheet'!DH20+'Questionnaire Analysis Sheet'!DI20)/'Questionnaire Analysis Sheet'!DD20)</f>
-        <v>0.18181818181818182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -13604,7 +13590,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21" s="13">
         <v>4</v>
@@ -13613,13 +13599,13 @@
         <v>4</v>
       </c>
       <c r="K21" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L21" s="13">
         <v>3</v>
       </c>
       <c r="M21" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N21" s="13">
         <v>4</v>
@@ -13724,7 +13710,7 @@
       <c r="DB21" s="13"/>
       <c r="DC21" s="14">
         <f t="shared" si="6"/>
-        <v>3.3636363636363638</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="DD21" s="15">
         <f t="shared" si="0"/>
@@ -13736,15 +13722,15 @@
       </c>
       <c r="DF21" s="28">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="DG21" s="28">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="DH21" s="28">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI21" s="28">
         <f t="shared" si="5"/>
@@ -13752,11 +13738,11 @@
       </c>
       <c r="DJ21" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE21+'Questionnaire Analysis Sheet'!DF21)/'Questionnaire Analysis Sheet'!DD21),"",('Questionnaire Analysis Sheet'!DE21+'Questionnaire Analysis Sheet'!DF21)/'Questionnaire Analysis Sheet'!DD21)</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="DK21" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH21+'Questionnaire Analysis Sheet'!DI21)/'Questionnaire Analysis Sheet'!DD21),"",('Questionnaire Analysis Sheet'!DH21+'Questionnaire Analysis Sheet'!DI21)/'Questionnaire Analysis Sheet'!DD21)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -13771,13 +13757,13 @@
       <c r="E22" s="89"/>
       <c r="F22" s="111"/>
       <c r="G22" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H22" s="13">
         <v>3</v>
       </c>
       <c r="I22" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J22" s="13">
         <v>4</v>
@@ -13894,7 +13880,7 @@
       <c r="DB22" s="13"/>
       <c r="DC22" s="14">
         <f t="shared" si="6"/>
-        <v>3.5454545454545454</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="DD22" s="15">
         <f t="shared" si="0"/>
@@ -13902,19 +13888,19 @@
       </c>
       <c r="DE22" s="28">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DF22" s="28">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DG22" s="28">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="DH22" s="28">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI22" s="28">
         <f t="shared" si="5"/>
@@ -13922,11 +13908,11 @@
       </c>
       <c r="DJ22" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DE22+'Questionnaire Analysis Sheet'!DF22)/'Questionnaire Analysis Sheet'!DD22),"",('Questionnaire Analysis Sheet'!DE22+'Questionnaire Analysis Sheet'!DF22)/'Questionnaire Analysis Sheet'!DD22)</f>
-        <v>0.54545454545454541</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="DK22" s="109">
         <f>IF(ISERROR(('Questionnaire Analysis Sheet'!DH22+'Questionnaire Analysis Sheet'!DI22)/'Questionnaire Analysis Sheet'!DD22),"",('Questionnaire Analysis Sheet'!DH22+'Questionnaire Analysis Sheet'!DI22)/'Questionnaire Analysis Sheet'!DD22)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:115" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -16712,15 +16698,15 @@
       <c r="F42" s="5"/>
       <c r="G42" s="14">
         <f>IF(ISERROR(AVERAGE(G15:G41)),"",AVERAGE(G15:G41))</f>
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="H42" s="14">
         <f t="shared" ref="H42:BS42" si="7">IF(ISERROR(AVERAGE(H15:H41)),"",AVERAGE(H15:H41))</f>
-        <v>3.5</v>
+        <v>4.25</v>
       </c>
       <c r="I42" s="14">
         <f t="shared" si="7"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="J42" s="14">
         <f t="shared" si="7"/>
@@ -16728,19 +16714,19 @@
       </c>
       <c r="K42" s="14">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>4.375</v>
       </c>
       <c r="L42" s="14">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M42" s="14">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>3.625</v>
       </c>
       <c r="N42" s="14">
         <f t="shared" si="7"/>
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="O42" s="14">
         <f t="shared" si="7"/>
@@ -16748,7 +16734,7 @@
       </c>
       <c r="P42" s="14">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>4.125</v>
       </c>
       <c r="Q42" s="14">
         <f t="shared" si="7"/>
@@ -17112,24 +17098,24 @@
       </c>
       <c r="DC42" s="80">
         <f t="shared" si="8"/>
-        <v>3.4545454545454546</v>
+        <v>3.9431818181818183</v>
       </c>
       <c r="DD42" s="72"/>
       <c r="DE42" s="73">
         <f>SUM(DE15:DE41)</f>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="DF42" s="73">
         <f t="shared" ref="DF42:DI42" si="9">SUM(DF15:DF41)</f>
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="DG42" s="73">
         <f t="shared" si="9"/>
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="DH42" s="73">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DI42" s="74">
         <f t="shared" si="9"/>
@@ -17434,10 +17420,10 @@
     <mergeCell ref="B10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="H11:DB13 G11:G14 G23:DB41 R15:DB22">
-    <cfRule type="cellIs" dxfId="10" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="302" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="303" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17478,18 +17464,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:Q18">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:Q22">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17518,7 +17504,7 @@
   <dimension ref="B2:T133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -17856,12 +17842,12 @@
       </c>
       <c r="H13" s="39">
         <f>'Questionnaire Analysis Sheet'!DC15</f>
-        <v>3.4545454545454546</v>
+        <v>3.8181818181818183</v>
       </c>
       <c r="I13" s="38"/>
       <c r="J13" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ15</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="K13" s="40">
         <f>'Questionnaire Analysis Sheet'!DK15</f>
@@ -17894,16 +17880,16 @@
       </c>
       <c r="H14" s="39">
         <f>'Questionnaire Analysis Sheet'!DC16</f>
-        <v>3.4545454545454546</v>
+        <v>4.0909090909090908</v>
       </c>
       <c r="I14" s="38"/>
       <c r="J14" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ16</f>
-        <v>0.45454545454545453</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="K14" s="40">
         <f>'Questionnaire Analysis Sheet'!DK16</f>
-        <v>0.18181818181818182</v>
+        <v>0</v>
       </c>
       <c r="L14" s="110"/>
       <c r="M14" s="41" t="str">
@@ -17932,16 +17918,16 @@
       </c>
       <c r="H15" s="39">
         <f>'Questionnaire Analysis Sheet'!DC17</f>
-        <v>3.3636363636363638</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="I15" s="38"/>
       <c r="J15" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ17</f>
-        <v>0.36363636363636365</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="K15" s="40">
         <f>'Questionnaire Analysis Sheet'!DK17</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
       <c r="L15" s="110"/>
       <c r="M15" s="41" t="str">
@@ -17970,16 +17956,16 @@
       </c>
       <c r="H16" s="39">
         <f>'Questionnaire Analysis Sheet'!DC18</f>
-        <v>3.5454545454545454</v>
+        <v>4</v>
       </c>
       <c r="I16" s="38"/>
       <c r="J16" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ18</f>
-        <v>0.54545454545454541</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="K16" s="40">
         <f>'Questionnaire Analysis Sheet'!DK18</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
       <c r="L16" s="110"/>
       <c r="M16" s="41" t="str">
@@ -18008,12 +17994,12 @@
       </c>
       <c r="H17" s="39">
         <f>'Questionnaire Analysis Sheet'!DC19</f>
-        <v>3.4545454545454546</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="I17" s="38"/>
       <c r="J17" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ19</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="K17" s="40">
         <f>'Questionnaire Analysis Sheet'!DK19</f>
@@ -18046,16 +18032,16 @@
       </c>
       <c r="H18" s="39">
         <f>'Questionnaire Analysis Sheet'!DC20</f>
-        <v>3.4545454545454546</v>
+        <v>4.3636363636363633</v>
       </c>
       <c r="I18" s="38"/>
       <c r="J18" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ20</f>
-        <v>0.45454545454545453</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="K18" s="40">
         <f>'Questionnaire Analysis Sheet'!DK20</f>
-        <v>0.18181818181818182</v>
+        <v>0</v>
       </c>
       <c r="L18" s="110"/>
       <c r="M18" s="41" t="str">
@@ -18084,16 +18070,16 @@
       </c>
       <c r="H19" s="39">
         <f>'Questionnaire Analysis Sheet'!DC21</f>
-        <v>3.3636363636363638</v>
+        <v>3.7272727272727271</v>
       </c>
       <c r="I19" s="38"/>
       <c r="J19" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ21</f>
-        <v>0.36363636363636365</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="K19" s="40">
         <f>'Questionnaire Analysis Sheet'!DK21</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
       <c r="L19" s="110"/>
       <c r="M19" s="41" t="str">
@@ -18122,16 +18108,16 @@
       </c>
       <c r="H20" s="39">
         <f>'Questionnaire Analysis Sheet'!DC22</f>
-        <v>3.5454545454545454</v>
+        <v>3.9090909090909092</v>
       </c>
       <c r="I20" s="38"/>
       <c r="J20" s="40">
         <f>'Questionnaire Analysis Sheet'!DJ22</f>
-        <v>0.54545454545454541</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="K20" s="40">
         <f>'Questionnaire Analysis Sheet'!DK22</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0</v>
       </c>
       <c r="L20" s="110"/>
       <c r="M20" s="41" t="str">
@@ -18877,7 +18863,7 @@
       <c r="G40" s="29"/>
       <c r="H40" s="102">
         <f>IF(ISERROR(AVERAGE(H13:H39)),"",AVERAGE(H13:H39))</f>
-        <v>3.4545454545454546</v>
+        <v>3.9431818181818183</v>
       </c>
       <c r="I40" s="103"/>
       <c r="J40" s="104"/>
@@ -19425,27 +19411,27 @@
       <c r="K67" s="33"/>
     </row>
     <row r="68" spans="2:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="122" t="s">
+      <c r="B68" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="C68" s="122"/>
-      <c r="D68" s="122"/>
-      <c r="E68" s="122"/>
-      <c r="F68" s="122"/>
-      <c r="G68" s="122"/>
-      <c r="H68" s="122"/>
-      <c r="I68" s="122"/>
-      <c r="J68" s="122"/>
-      <c r="K68" s="122"/>
-      <c r="L68" s="122"/>
-      <c r="M68" s="122"/>
-      <c r="N68" s="122"/>
-      <c r="O68" s="122"/>
-      <c r="P68" s="122"/>
-      <c r="Q68" s="122"/>
-      <c r="R68" s="122"/>
-      <c r="S68" s="122"/>
-      <c r="T68" s="122"/>
+      <c r="C68" s="123"/>
+      <c r="D68" s="123"/>
+      <c r="E68" s="123"/>
+      <c r="F68" s="123"/>
+      <c r="G68" s="123"/>
+      <c r="H68" s="123"/>
+      <c r="I68" s="123"/>
+      <c r="J68" s="123"/>
+      <c r="K68" s="123"/>
+      <c r="L68" s="123"/>
+      <c r="M68" s="123"/>
+      <c r="N68" s="123"/>
+      <c r="O68" s="123"/>
+      <c r="P68" s="123"/>
+      <c r="Q68" s="123"/>
+      <c r="R68" s="123"/>
+      <c r="S68" s="123"/>
+      <c r="T68" s="123"/>
     </row>
     <row r="69" spans="2:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="35"/>
@@ -19699,10 +19685,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13:M40">
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
       <formula>"p"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19815,7 +19801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:S9 C5:F9">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>